<commit_message>
Fix links, correct label in spreadsheet
</commit_message>
<xml_diff>
--- a/data/Spain.Legacy/Content/Legacy HeatCalculator.xlsx
+++ b/data/Spain.Legacy/Content/Legacy HeatCalculator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ianmayo/git/LegacyMan/data/Britain_Cmplx/Content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ian/git/LegacyMan/data/Spain.Legacy/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B73BA3-03BF-6648-B270-FDD9E76848AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2990ED75-606F-7C4E-9B63-5F1A4ACC5CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" xr2:uid="{A7AC6855-1DA2-3545-8A73-D5FBF8017C5B}"/>
   </bookViews>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -50,7 +49,7 @@
     <t>Rate:</t>
   </si>
   <si>
-    <t>BRITAIN COMPLEX</t>
+    <t>SPAIN LEGACY</t>
   </si>
 </sst>
 </file>

</xml_diff>